<commit_message>
Arreglo validacion localizador mandatory y agrego data para QA. Comienzo validacion de suma asegurada
</commit_message>
<xml_diff>
--- a/Sura/Validación de Localizador - Emisión.xlsx
+++ b/Sura/Validación de Localizador - Emisión.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DF1901-3316-4858-AC02-67FE8980DE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1323C602-3972-42E7-8CEA-5D199E774E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="78">
   <si>
     <t>Usuario</t>
   </si>
@@ -223,6 +223,42 @@
   </si>
   <si>
     <t>TipoValidacion</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/pc/PolicyCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
+  </si>
+  <si>
+    <t>gw</t>
+  </si>
+  <si>
+    <t>3582596139</t>
+  </si>
+  <si>
+    <t>D-40</t>
+  </si>
+  <si>
+    <t>1.500.000</t>
+  </si>
+  <si>
+    <t>MMM130</t>
+  </si>
+  <si>
+    <t>MASDAS12331</t>
+  </si>
+  <si>
+    <t>ASDAKE1251</t>
+  </si>
+  <si>
+    <t>MMM131</t>
+  </si>
+  <si>
+    <t>MASDAS12332</t>
+  </si>
+  <si>
+    <t>ASDAKE1252</t>
   </si>
 </sst>
 </file>
@@ -290,8 +326,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -575,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +627,7 @@
     <col min="10" max="10" width="14.85546875" customWidth="1"/>
     <col min="11" max="12" width="21.28515625" customWidth="1"/>
     <col min="13" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
     <col min="15" max="15" width="7.85546875" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" customWidth="1"/>
     <col min="17" max="17" width="22.42578125" customWidth="1"/>
@@ -679,7 +715,7 @@
       <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F2" t="s">
@@ -741,7 +777,7 @@
       <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F3" t="s">
@@ -803,7 +839,7 @@
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F4" t="s">
@@ -865,7 +901,7 @@
       <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F5" t="s">
@@ -927,7 +963,7 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F6" t="s">
@@ -989,7 +1025,7 @@
       <c r="D7" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F7" t="s">
@@ -1051,7 +1087,7 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F8" t="s">
@@ -1101,20 +1137,194 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>2022</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>40</v>
+      </c>
+      <c r="R9" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="E10" s="4"/>
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10">
+        <v>2022</v>
+      </c>
+      <c r="N10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P10">
+        <v>999000</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>40</v>
+      </c>
+      <c r="R10" t="s">
+        <v>72</v>
+      </c>
+      <c r="S10" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="E11" s="1"/>
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11">
+        <v>2022</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>40</v>
+      </c>
+      <c r="R11" t="s">
+        <v>75</v>
+      </c>
+      <c r="S11" t="s">
+        <v>76</v>
+      </c>
+      <c r="T11" t="s">
+        <v>77</v>
+      </c>
+      <c r="U11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>

</xml_diff>